<commit_message>
implement upload file with student list, api get grade board, map student to grade board
</commit_message>
<xml_diff>
--- a/public/assets/export-template/export-student-template.xlsx
+++ b/public/assets/export-template/export-student-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\final year\web 2\midterm\Advanced-Web-BE\public\assets\export-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575E7443-3092-4BA5-8A5D-0CAAD88A2709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBE99B1-1913-404D-BCD1-0ABF01FECBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,52 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>SĐT</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve">Họ tên </t>
   </si>
   <si>
-    <t>Ngày sinh</t>
-  </si>
-  <si>
-    <t>format dd/mm/yyyy</t>
-  </si>
-  <si>
-    <t>VD: PS333</t>
-  </si>
-  <si>
-    <t>VD: Nguyễn Văn A</t>
-  </si>
-  <si>
-    <t>VD: 24/12/1995</t>
-  </si>
-  <si>
-    <t>VD: 0456123789</t>
-  </si>
-  <si>
-    <t>VD: nguyenvanabc@gmail.com</t>
-  </si>
-  <si>
-    <t>CMND/CCCD</t>
-  </si>
-  <si>
-    <t>VD: 251226432</t>
-  </si>
-  <si>
     <t>Mã</t>
-  </si>
-  <si>
-    <t>Không được bỏ trống</t>
-  </si>
-  <si>
-    <t>Không được bỏ trống trường này
-Đảm bảo rằng mã là duy nhất.</t>
   </si>
 </sst>
 </file>
@@ -94,7 +54,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,26 +67,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8EA9DB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -149,34 +91,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,88 +386,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0832A9C-4272-4666-B7B2-EC79D568A3C5}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" style="4" customWidth="1"/>
-    <col min="2" max="2" width="37.28515625" style="4" customWidth="1"/>
-    <col min="3" max="4" width="20.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="20" style="4" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="37.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A3:F3"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implement export grade board
</commit_message>
<xml_diff>
--- a/public/assets/export-template/export-student-template.xlsx
+++ b/public/assets/export-template/export-student-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\final year\web 2\midterm\Advanced-Web-BE\public\assets\export-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBE99B1-1913-404D-BCD1-0ABF01FECBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CB47AA-F955-44AA-9026-222FF019F4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="student" sheetId="2" r:id="rId1"/>
@@ -389,12 +389,12 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="26" style="2" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>

</xml_diff>